<commit_message>
adicionando dba e anal infra
</commit_message>
<xml_diff>
--- a/EDSI/Cargos Projeto EDS.xlsx
+++ b/EDSI/Cargos Projeto EDS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Cargo</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Analista Programador</t>
+  </si>
+  <si>
+    <t>DBA</t>
+  </si>
+  <si>
+    <t>Analista de Infra</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D7" si="0">B3*168*C3</f>
+        <f t="shared" ref="D3:D9" si="0">B3*168*C3</f>
         <v>8904</v>
       </c>
     </row>
@@ -527,8 +533,41 @@
         <v>6384</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>11760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>6216</v>
+      </c>
+    </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>